<commit_message>
e05 done - final commit
</commit_message>
<xml_diff>
--- a/ex05.xlsx
+++ b/ex05.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CSE\CSMC\ex05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA7FEA6-1F19-44CF-9D05-6CCFF0D81CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBA7E18-4D67-4DC2-9EE6-383714BD846B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="19140" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="P1" sheetId="1" r:id="rId1"/>
+    <sheet name="P2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>N</t>
   </si>
@@ -70,6 +71,60 @@
   </si>
   <si>
     <t>custom k=32</t>
+  </si>
+  <si>
+    <t>ppd</t>
+  </si>
+  <si>
+    <t>N_unknowns</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>pipelined</t>
+  </si>
+  <si>
+    <t>0.02194 (0.000467532 per iteration)</t>
+  </si>
+  <si>
+    <t>0.023167 (0.000494106 per iteration)</t>
+  </si>
+  <si>
+    <t>0.046154 (0.000491255 per iteration)</t>
+  </si>
+  <si>
+    <t>0.043654 (0.000464798 per iteration)</t>
+  </si>
+  <si>
+    <t>0.095537 (0.000502968 per iteration)</t>
+  </si>
+  <si>
+    <t>0.091164 (0.000479974 per iteration)</t>
+  </si>
+  <si>
+    <t>0.238176 (0.000620372 per iteration)</t>
+  </si>
+  <si>
+    <t>0.232374 (0.000605247 per iteration)</t>
+  </si>
+  <si>
+    <t>0.776221 (0.00100163 per iteration)</t>
+  </si>
+  <si>
+    <t>0.767084 (0.000989821 per iteration)</t>
+  </si>
+  <si>
+    <t>1.91527 (0.00122383 per iteration)</t>
+  </si>
+  <si>
+    <t>1.7684 (0.00112998 per iteration)</t>
+  </si>
+  <si>
+    <t>9.24658 (0.00292522 per iteration)</t>
+  </si>
+  <si>
+    <t>7.82304 (0.00247487 per iteration)</t>
   </si>
 </sst>
 </file>
@@ -168,7 +223,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$I$3</c:f>
+              <c:f>'P1'!$I$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -192,7 +247,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -228,7 +283,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$4:$I$12</c:f>
+              <c:f>'P1'!$I$4:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -274,7 +329,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$3</c:f>
+              <c:f>'P1'!$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -298,7 +353,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -334,7 +389,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$4:$J$12</c:f>
+              <c:f>'P1'!$J$4:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -380,7 +435,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$I$14</c:f>
+              <c:f>'P1'!$I$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -407,7 +462,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -443,7 +498,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$15:$I$23</c:f>
+              <c:f>'P1'!$I$15:$I$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -489,7 +544,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$14</c:f>
+              <c:f>'P1'!$J$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -516,7 +571,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -552,7 +607,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$15:$J$23</c:f>
+              <c:f>'P1'!$J$15:$J$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -598,7 +653,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$I$25</c:f>
+              <c:f>'P1'!$I$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -621,7 +676,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -657,7 +712,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$26:$I$34</c:f>
+              <c:f>'P1'!$I$26:$I$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -703,7 +758,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$25</c:f>
+              <c:f>'P1'!$J$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -726,7 +781,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -762,7 +817,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$26:$J$34</c:f>
+              <c:f>'P1'!$J$26:$J$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -808,7 +863,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$I$36</c:f>
+              <c:f>'P1'!$I$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -834,7 +889,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -870,7 +925,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$37:$I$45</c:f>
+              <c:f>'P1'!$I$37:$I$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -916,7 +971,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$36</c:f>
+              <c:f>'P1'!$J$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -942,7 +997,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -978,7 +1033,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$37:$J$45</c:f>
+              <c:f>'P1'!$J$37:$J$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1336,7 +1391,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$36</c:f>
+              <c:f>'P1'!$J$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1360,7 +1415,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1396,7 +1451,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$37:$J$45</c:f>
+              <c:f>'P1'!$J$37:$J$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1442,7 +1497,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$25</c:f>
+              <c:f>'P1'!$J$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1464,7 +1519,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1500,7 +1555,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$26:$J$34</c:f>
+              <c:f>'P1'!$J$26:$J$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1546,7 +1601,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$14</c:f>
+              <c:f>'P1'!$J$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1570,7 +1625,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1606,7 +1661,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$15:$J$23</c:f>
+              <c:f>'P1'!$J$15:$J$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1652,7 +1707,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$3</c:f>
+              <c:f>'P1'!$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1674,7 +1729,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1710,7 +1765,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$4:$J$12</c:f>
+              <c:f>'P1'!$J$4:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1772,7 +1827,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$3</c15:sqref>
+                          <c15:sqref>'P1'!$I$3</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1802,7 +1857,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$H$4:$H$12</c15:sqref>
+                          <c15:sqref>'P1'!$H$4:$H$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1844,7 +1899,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$4:$I$12</c15:sqref>
+                          <c15:sqref>'P1'!$I$4:$I$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1895,10 +1950,10 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$14</c15:sqref>
+                          <c15:sqref>'P1'!$I$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1928,10 +1983,10 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$H$4:$H$12</c15:sqref>
+                          <c15:sqref>'P1'!$H$4:$H$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1970,10 +2025,10 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$15:$I$23</c15:sqref>
+                          <c15:sqref>'P1'!$I$15:$I$23</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2011,7 +2066,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-B84C-45F3-B352-1FA93C6C7337}"/>
                   </c:ext>
@@ -2024,10 +2079,10 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$25</c15:sqref>
+                          <c15:sqref>'P1'!$I$25</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2053,10 +2108,10 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$H$4:$H$12</c15:sqref>
+                          <c15:sqref>'P1'!$H$4:$H$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2095,10 +2150,10 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$26:$I$34</c15:sqref>
+                          <c15:sqref>'P1'!$I$26:$I$34</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2136,7 +2191,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-B84C-45F3-B352-1FA93C6C7337}"/>
                   </c:ext>
@@ -2149,10 +2204,10 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$36</c15:sqref>
+                          <c15:sqref>'P1'!$I$36</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2181,10 +2236,10 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$H$4:$H$12</c15:sqref>
+                          <c15:sqref>'P1'!$H$4:$H$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2223,10 +2278,10 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$37:$I$45</c15:sqref>
+                          <c15:sqref>'P1'!$I$37:$I$45</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2264,7 +2319,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-B84C-45F3-B352-1FA93C6C7337}"/>
                   </c:ext>
@@ -2580,7 +2635,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$I$36</c:f>
+              <c:f>'P1'!$I$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2607,7 +2662,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2644,7 +2699,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$37:$I$45</c:f>
+              <c:f>'P1'!$I$37:$I$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2691,7 +2746,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$36</c:f>
+              <c:f>'P1'!$J$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2715,7 +2770,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2751,7 +2806,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$37:$J$45</c:f>
+              <c:f>'P1'!$J$37:$J$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2797,7 +2852,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$I$3</c:f>
+              <c:f>'P1'!$I$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2822,7 +2877,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2859,7 +2914,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$4:$I$12</c:f>
+              <c:f>'P1'!$I$4:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2906,7 +2961,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$J$3</c:f>
+              <c:f>'P1'!$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2928,7 +2983,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$H$4:$H$12</c:f>
+              <c:f>'P1'!$H$4:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2964,7 +3019,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$J$4:$J$12</c:f>
+              <c:f>'P1'!$J$4:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3026,7 +3081,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$J$25</c15:sqref>
+                          <c15:sqref>'P1'!$J$25</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3054,7 +3109,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$H$4:$H$12</c15:sqref>
+                          <c15:sqref>'P1'!$H$4:$H$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3096,7 +3151,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$J$26:$J$34</c15:sqref>
+                          <c15:sqref>'P1'!$J$26:$J$34</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3147,10 +3202,10 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$J$14</c15:sqref>
+                          <c15:sqref>'P1'!$J$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3177,10 +3232,10 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$H$4:$H$12</c15:sqref>
+                          <c15:sqref>'P1'!$H$4:$H$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3219,10 +3274,10 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$J$15:$J$23</c15:sqref>
+                          <c15:sqref>'P1'!$J$15:$J$23</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3260,7 +3315,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-5003-4768-BEBD-BEC89E075FBD}"/>
                   </c:ext>
@@ -3276,7 +3331,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$14</c15:sqref>
+                          <c15:sqref>'P1'!$I$14</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3309,7 +3364,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$H$4:$H$12</c15:sqref>
+                          <c15:sqref>'P1'!$H$4:$H$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3351,7 +3406,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$15:$I$23</c15:sqref>
+                          <c15:sqref>'P1'!$I$15:$I$23</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3405,7 +3460,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$25</c15:sqref>
+                          <c15:sqref>'P1'!$I$25</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3434,7 +3489,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$H$4:$H$12</c15:sqref>
+                          <c15:sqref>'P1'!$H$4:$H$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3476,7 +3531,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Tabelle1!$I$26:$I$34</c15:sqref>
+                          <c15:sqref>'P1'!$I$26:$I$34</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4177,7 +4232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
@@ -5282,4 +5337,148 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E478ACA1-BA2F-4304-91D5-2EF3ED49FCD7}">
+  <dimension ref="A3:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <f>A4^2</f>
+        <v>900</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <f>A4*2</f>
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B10" si="0">A5^2</f>
+        <v>3600</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <f t="shared" ref="A6:A20" si="1">A5*2</f>
+        <v>120</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>14400</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>57600</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>230400</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>960</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>921600</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>1920</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>3686400</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>